<commit_message>
filter entities based on existing entities in jar file
</commit_message>
<xml_diff>
--- a/results/keyclasses_results.xlsx
+++ b/results/keyclasses_results.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="overview" sheetId="1" r:id="rId1"/>
+    <sheet name="results" sheetId="2" r:id="rId2"/>
+    <sheet name="commit statistics" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="119">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -336,6 +337,42 @@
   </si>
   <si>
     <t>v1.6.3</t>
+  </si>
+  <si>
+    <t>&lt; 5 files</t>
+  </si>
+  <si>
+    <t>&gt;5 &lt;10 files</t>
+  </si>
+  <si>
+    <t>&gt;20 files</t>
+  </si>
+  <si>
+    <t>&gt;10 &lt;20 files</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>jhotdraw</t>
+  </si>
+  <si>
+    <t>tomcat</t>
+  </si>
+  <si>
+    <t>C: Nr of commits with less than 5 files</t>
+  </si>
+  <si>
+    <t>D: Nr of commits with more than 5 and less then 10 files</t>
+  </si>
+  <si>
+    <t>E: Nr of commits with more than 10 and less then 20 files</t>
+  </si>
+  <si>
+    <t>F: Nr of commits with more than 20 files</t>
+  </si>
+  <si>
+    <t>G: Average nr of files/commit</t>
   </si>
 </sst>
 </file>
@@ -849,6 +886,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -858,6 +907,27 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -867,13 +937,43 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -882,70 +982,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1255,8 +1292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1861,7 +1898,7 @@
   <dimension ref="A1:CZ9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1886,220 +1923,220 @@
       <c r="F2" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="72" t="s">
+      <c r="G2" s="69" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="73"/>
-      <c r="U2" s="74"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="70"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="71"/>
       <c r="V2" s="49"/>
-      <c r="W2" s="75" t="s">
+      <c r="W2" s="72" t="s">
         <v>74</v>
       </c>
-      <c r="X2" s="63"/>
-      <c r="Y2" s="63"/>
-      <c r="Z2" s="63"/>
-      <c r="AA2" s="63"/>
-      <c r="AB2" s="63"/>
-      <c r="AC2" s="63"/>
-      <c r="AD2" s="63"/>
-      <c r="AE2" s="63"/>
-      <c r="AF2" s="63"/>
-      <c r="AG2" s="63"/>
-      <c r="AH2" s="63"/>
-      <c r="AI2" s="63"/>
-      <c r="AJ2" s="63"/>
-      <c r="AK2" s="63"/>
-      <c r="AL2" s="76"/>
-      <c r="AM2" s="77" t="s">
+      <c r="X2" s="52"/>
+      <c r="Y2" s="52"/>
+      <c r="Z2" s="52"/>
+      <c r="AA2" s="52"/>
+      <c r="AB2" s="52"/>
+      <c r="AC2" s="52"/>
+      <c r="AD2" s="52"/>
+      <c r="AE2" s="52"/>
+      <c r="AF2" s="52"/>
+      <c r="AG2" s="52"/>
+      <c r="AH2" s="52"/>
+      <c r="AI2" s="52"/>
+      <c r="AJ2" s="52"/>
+      <c r="AK2" s="52"/>
+      <c r="AL2" s="73"/>
+      <c r="AM2" s="74" t="s">
         <v>75</v>
       </c>
-      <c r="AN2" s="63"/>
-      <c r="AO2" s="63"/>
-      <c r="AP2" s="63"/>
-      <c r="AQ2" s="63"/>
-      <c r="AR2" s="63"/>
-      <c r="AS2" s="63"/>
-      <c r="AT2" s="63"/>
-      <c r="AU2" s="63"/>
-      <c r="AV2" s="63"/>
-      <c r="AW2" s="63"/>
-      <c r="AX2" s="63"/>
-      <c r="AY2" s="63"/>
-      <c r="AZ2" s="63"/>
-      <c r="BA2" s="63"/>
-      <c r="BB2" s="63"/>
-      <c r="BC2" s="63" t="s">
+      <c r="AN2" s="52"/>
+      <c r="AO2" s="52"/>
+      <c r="AP2" s="52"/>
+      <c r="AQ2" s="52"/>
+      <c r="AR2" s="52"/>
+      <c r="AS2" s="52"/>
+      <c r="AT2" s="52"/>
+      <c r="AU2" s="52"/>
+      <c r="AV2" s="52"/>
+      <c r="AW2" s="52"/>
+      <c r="AX2" s="52"/>
+      <c r="AY2" s="52"/>
+      <c r="AZ2" s="52"/>
+      <c r="BA2" s="52"/>
+      <c r="BB2" s="52"/>
+      <c r="BC2" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="BD2" s="63"/>
-      <c r="BE2" s="63"/>
-      <c r="BF2" s="63"/>
-      <c r="BG2" s="63"/>
-      <c r="BH2" s="63"/>
-      <c r="BI2" s="63"/>
-      <c r="BJ2" s="63"/>
-      <c r="BK2" s="63"/>
-      <c r="BL2" s="63"/>
-      <c r="BM2" s="63"/>
-      <c r="BN2" s="63"/>
-      <c r="BO2" s="63"/>
-      <c r="BP2" s="63"/>
-      <c r="BQ2" s="63"/>
-      <c r="BR2" s="63"/>
-      <c r="BS2" s="63" t="s">
+      <c r="BD2" s="52"/>
+      <c r="BE2" s="52"/>
+      <c r="BF2" s="52"/>
+      <c r="BG2" s="52"/>
+      <c r="BH2" s="52"/>
+      <c r="BI2" s="52"/>
+      <c r="BJ2" s="52"/>
+      <c r="BK2" s="52"/>
+      <c r="BL2" s="52"/>
+      <c r="BM2" s="52"/>
+      <c r="BN2" s="52"/>
+      <c r="BO2" s="52"/>
+      <c r="BP2" s="52"/>
+      <c r="BQ2" s="52"/>
+      <c r="BR2" s="52"/>
+      <c r="BS2" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="BT2" s="63"/>
-      <c r="BU2" s="63"/>
-      <c r="BV2" s="63"/>
-      <c r="BW2" s="63"/>
-      <c r="BX2" s="63"/>
-      <c r="BY2" s="63"/>
-      <c r="BZ2" s="63"/>
-      <c r="CA2" s="63"/>
-      <c r="CB2" s="63"/>
-      <c r="CC2" s="63"/>
-      <c r="CD2" s="63"/>
-      <c r="CE2" s="63"/>
-      <c r="CF2" s="63"/>
-      <c r="CG2" s="63"/>
-      <c r="CH2" s="63"/>
+      <c r="BT2" s="52"/>
+      <c r="BU2" s="52"/>
+      <c r="BV2" s="52"/>
+      <c r="BW2" s="52"/>
+      <c r="BX2" s="52"/>
+      <c r="BY2" s="52"/>
+      <c r="BZ2" s="52"/>
+      <c r="CA2" s="52"/>
+      <c r="CB2" s="52"/>
+      <c r="CC2" s="52"/>
+      <c r="CD2" s="52"/>
+      <c r="CE2" s="52"/>
+      <c r="CF2" s="52"/>
+      <c r="CG2" s="52"/>
+      <c r="CH2" s="52"/>
       <c r="CI2" s="50"/>
     </row>
     <row r="3" spans="1:104" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F3" s="18"/>
-      <c r="G3" s="64" t="s">
+      <c r="G3" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="52" t="s">
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="67" t="s">
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="P3" s="67"/>
-      <c r="Q3" s="67"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
       <c r="R3" s="19"/>
-      <c r="S3" s="58" t="s">
+      <c r="S3" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="T3" s="59"/>
-      <c r="U3" s="59"/>
-      <c r="V3" s="68"/>
-      <c r="W3" s="69" t="s">
+      <c r="T3" s="61"/>
+      <c r="U3" s="61"/>
+      <c r="V3" s="62"/>
+      <c r="W3" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="X3" s="70"/>
-      <c r="Y3" s="70"/>
-      <c r="Z3" s="71"/>
-      <c r="AA3" s="74" t="s">
+      <c r="X3" s="64"/>
+      <c r="Y3" s="64"/>
+      <c r="Z3" s="65"/>
+      <c r="AA3" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="AB3" s="78"/>
-      <c r="AC3" s="78"/>
-      <c r="AD3" s="72"/>
-      <c r="AE3" s="79" t="s">
+      <c r="AB3" s="75"/>
+      <c r="AC3" s="75"/>
+      <c r="AD3" s="69"/>
+      <c r="AE3" s="76" t="s">
         <v>80</v>
       </c>
-      <c r="AF3" s="80"/>
-      <c r="AG3" s="80"/>
-      <c r="AH3" s="81"/>
-      <c r="AI3" s="82" t="s">
+      <c r="AF3" s="77"/>
+      <c r="AG3" s="77"/>
+      <c r="AH3" s="78"/>
+      <c r="AI3" s="79" t="s">
         <v>81</v>
       </c>
-      <c r="AJ3" s="83"/>
-      <c r="AK3" s="83"/>
-      <c r="AL3" s="83"/>
-      <c r="AM3" s="84" t="s">
+      <c r="AJ3" s="80"/>
+      <c r="AK3" s="80"/>
+      <c r="AL3" s="80"/>
+      <c r="AM3" s="81" t="s">
         <v>78</v>
       </c>
-      <c r="AN3" s="61"/>
-      <c r="AO3" s="61"/>
-      <c r="AP3" s="62"/>
-      <c r="AQ3" s="52" t="s">
+      <c r="AN3" s="82"/>
+      <c r="AO3" s="82"/>
+      <c r="AP3" s="83"/>
+      <c r="AQ3" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="AR3" s="53"/>
-      <c r="AS3" s="53"/>
-      <c r="AT3" s="54"/>
-      <c r="AU3" s="55" t="s">
+      <c r="AR3" s="57"/>
+      <c r="AS3" s="57"/>
+      <c r="AT3" s="58"/>
+      <c r="AU3" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="AV3" s="56"/>
-      <c r="AW3" s="56"/>
-      <c r="AX3" s="57"/>
-      <c r="AY3" s="58" t="s">
+      <c r="AV3" s="67"/>
+      <c r="AW3" s="67"/>
+      <c r="AX3" s="68"/>
+      <c r="AY3" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="AZ3" s="59"/>
-      <c r="BA3" s="59"/>
-      <c r="BB3" s="59"/>
-      <c r="BC3" s="61" t="s">
+      <c r="AZ3" s="61"/>
+      <c r="BA3" s="61"/>
+      <c r="BB3" s="61"/>
+      <c r="BC3" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="BD3" s="61"/>
-      <c r="BE3" s="61"/>
-      <c r="BF3" s="62"/>
-      <c r="BG3" s="52" t="s">
+      <c r="BD3" s="82"/>
+      <c r="BE3" s="82"/>
+      <c r="BF3" s="83"/>
+      <c r="BG3" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="BH3" s="53"/>
-      <c r="BI3" s="53"/>
-      <c r="BJ3" s="54"/>
-      <c r="BK3" s="55" t="s">
+      <c r="BH3" s="57"/>
+      <c r="BI3" s="57"/>
+      <c r="BJ3" s="58"/>
+      <c r="BK3" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="BL3" s="56"/>
-      <c r="BM3" s="56"/>
-      <c r="BN3" s="57"/>
-      <c r="BO3" s="58" t="s">
+      <c r="BL3" s="67"/>
+      <c r="BM3" s="67"/>
+      <c r="BN3" s="68"/>
+      <c r="BO3" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="BP3" s="59"/>
-      <c r="BQ3" s="59"/>
-      <c r="BR3" s="59"/>
-      <c r="BS3" s="61" t="s">
+      <c r="BP3" s="61"/>
+      <c r="BQ3" s="61"/>
+      <c r="BR3" s="61"/>
+      <c r="BS3" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="BT3" s="61"/>
-      <c r="BU3" s="61"/>
-      <c r="BV3" s="62"/>
-      <c r="BW3" s="52" t="s">
+      <c r="BT3" s="82"/>
+      <c r="BU3" s="82"/>
+      <c r="BV3" s="83"/>
+      <c r="BW3" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="BX3" s="53"/>
-      <c r="BY3" s="53"/>
-      <c r="BZ3" s="54"/>
-      <c r="CA3" s="55" t="s">
+      <c r="BX3" s="57"/>
+      <c r="BY3" s="57"/>
+      <c r="BZ3" s="58"/>
+      <c r="CA3" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="CB3" s="56"/>
-      <c r="CC3" s="56"/>
-      <c r="CD3" s="57"/>
-      <c r="CE3" s="58" t="s">
+      <c r="CB3" s="67"/>
+      <c r="CC3" s="67"/>
+      <c r="CD3" s="68"/>
+      <c r="CE3" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="CF3" s="59"/>
-      <c r="CG3" s="59"/>
-      <c r="CH3" s="60"/>
+      <c r="CF3" s="61"/>
+      <c r="CG3" s="61"/>
+      <c r="CH3" s="84"/>
       <c r="CI3" s="16"/>
     </row>
     <row r="4" spans="1:104" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -3748,6 +3785,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="BW3:BZ3"/>
+    <mergeCell ref="CA3:CD3"/>
+    <mergeCell ref="CE3:CH3"/>
+    <mergeCell ref="AY3:BB3"/>
+    <mergeCell ref="BC3:BF3"/>
+    <mergeCell ref="BG3:BJ3"/>
+    <mergeCell ref="BK3:BN3"/>
+    <mergeCell ref="BO3:BR3"/>
+    <mergeCell ref="BS3:BV3"/>
     <mergeCell ref="BS2:CH2"/>
     <mergeCell ref="G3:J3"/>
     <mergeCell ref="K3:N3"/>
@@ -3764,15 +3810,6 @@
     <mergeCell ref="AI3:AL3"/>
     <mergeCell ref="AM3:AP3"/>
     <mergeCell ref="AQ3:AT3"/>
-    <mergeCell ref="BW3:BZ3"/>
-    <mergeCell ref="CA3:CD3"/>
-    <mergeCell ref="CE3:CH3"/>
-    <mergeCell ref="AY3:BB3"/>
-    <mergeCell ref="BC3:BF3"/>
-    <mergeCell ref="BG3:BJ3"/>
-    <mergeCell ref="BK3:BN3"/>
-    <mergeCell ref="BO3:BR3"/>
-    <mergeCell ref="BS3:BV3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="CJ5" r:id="rId1"/>
@@ -3783,4 +3820,222 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A5:J12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="54.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="30">
+        <v>1</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6">
+        <v>3856</v>
+      </c>
+      <c r="D6">
+        <v>345</v>
+      </c>
+      <c r="E6">
+        <v>192</v>
+      </c>
+      <c r="F6">
+        <v>208</v>
+      </c>
+      <c r="G6">
+        <v>5.81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="30">
+        <v>2</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7">
+        <v>3770</v>
+      </c>
+      <c r="D7">
+        <v>650</v>
+      </c>
+      <c r="E7">
+        <v>394</v>
+      </c>
+      <c r="F7">
+        <v>441</v>
+      </c>
+      <c r="G7">
+        <v>11.98</v>
+      </c>
+      <c r="J7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="30">
+        <v>3</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8">
+        <v>1428</v>
+      </c>
+      <c r="D8">
+        <v>91</v>
+      </c>
+      <c r="E8">
+        <v>52</v>
+      </c>
+      <c r="F8">
+        <v>59</v>
+      </c>
+      <c r="G8">
+        <v>3.82</v>
+      </c>
+      <c r="J8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="30">
+        <v>4</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9">
+        <v>331</v>
+      </c>
+      <c r="D9">
+        <v>45</v>
+      </c>
+      <c r="E9">
+        <v>21</v>
+      </c>
+      <c r="F9">
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <v>4.32</v>
+      </c>
+      <c r="J9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="30">
+        <v>5</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10">
+        <v>1640</v>
+      </c>
+      <c r="D10">
+        <v>302</v>
+      </c>
+      <c r="E10">
+        <v>153</v>
+      </c>
+      <c r="F10">
+        <v>94</v>
+      </c>
+      <c r="G10">
+        <v>5.46</v>
+      </c>
+      <c r="J10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="30">
+        <v>6</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11">
+        <v>91</v>
+      </c>
+      <c r="D11">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>26</v>
+      </c>
+      <c r="G11">
+        <v>32.89</v>
+      </c>
+      <c r="J11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="30">
+        <v>7</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12">
+        <v>13579</v>
+      </c>
+      <c r="D12">
+        <v>812</v>
+      </c>
+      <c r="E12">
+        <v>304</v>
+      </c>
+      <c r="F12">
+        <v>236</v>
+      </c>
+      <c r="G12">
+        <v>2.89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
filter commits by given threshold
</commit_message>
<xml_diff>
--- a/results/keyclasses_results.xlsx
+++ b/results/keyclasses_results.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2206" uniqueCount="1993">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2221" uniqueCount="1997">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -6000,6 +6000,18 @@
   </si>
   <si>
     <t>Jar - Extracted from git code (Is in jar but not in git code) Count: 803</t>
+  </si>
+  <si>
+    <t>1 occ</t>
+  </si>
+  <si>
+    <t>2 occ</t>
+  </si>
+  <si>
+    <t>3 occ</t>
+  </si>
+  <si>
+    <t>4 occ</t>
   </si>
 </sst>
 </file>
@@ -6530,6 +6542,39 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6542,22 +6587,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6570,15 +6600,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6618,15 +6639,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7539,10 +7551,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DA21"/>
+  <dimension ref="A1:DA29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7571,221 +7583,221 @@
       <c r="G2" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="H2" s="74" t="s">
+      <c r="H2" s="77" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="75"/>
-      <c r="S2" s="75"/>
-      <c r="T2" s="75"/>
-      <c r="U2" s="75"/>
-      <c r="V2" s="76"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="78"/>
+      <c r="T2" s="78"/>
+      <c r="U2" s="78"/>
+      <c r="V2" s="79"/>
       <c r="W2" s="49"/>
-      <c r="X2" s="77" t="s">
+      <c r="X2" s="80" t="s">
         <v>74</v>
       </c>
-      <c r="Y2" s="57"/>
-      <c r="Z2" s="57"/>
-      <c r="AA2" s="57"/>
-      <c r="AB2" s="57"/>
-      <c r="AC2" s="57"/>
-      <c r="AD2" s="57"/>
-      <c r="AE2" s="57"/>
-      <c r="AF2" s="57"/>
-      <c r="AG2" s="57"/>
-      <c r="AH2" s="57"/>
-      <c r="AI2" s="57"/>
-      <c r="AJ2" s="57"/>
-      <c r="AK2" s="57"/>
-      <c r="AL2" s="57"/>
-      <c r="AM2" s="78"/>
-      <c r="AN2" s="79" t="s">
+      <c r="Y2" s="68"/>
+      <c r="Z2" s="68"/>
+      <c r="AA2" s="68"/>
+      <c r="AB2" s="68"/>
+      <c r="AC2" s="68"/>
+      <c r="AD2" s="68"/>
+      <c r="AE2" s="68"/>
+      <c r="AF2" s="68"/>
+      <c r="AG2" s="68"/>
+      <c r="AH2" s="68"/>
+      <c r="AI2" s="68"/>
+      <c r="AJ2" s="68"/>
+      <c r="AK2" s="68"/>
+      <c r="AL2" s="68"/>
+      <c r="AM2" s="81"/>
+      <c r="AN2" s="82" t="s">
         <v>75</v>
       </c>
-      <c r="AO2" s="57"/>
-      <c r="AP2" s="57"/>
-      <c r="AQ2" s="57"/>
-      <c r="AR2" s="57"/>
-      <c r="AS2" s="57"/>
-      <c r="AT2" s="57"/>
-      <c r="AU2" s="57"/>
-      <c r="AV2" s="57"/>
-      <c r="AW2" s="57"/>
-      <c r="AX2" s="57"/>
-      <c r="AY2" s="57"/>
-      <c r="AZ2" s="57"/>
-      <c r="BA2" s="57"/>
-      <c r="BB2" s="57"/>
-      <c r="BC2" s="57"/>
-      <c r="BD2" s="57" t="s">
+      <c r="AO2" s="68"/>
+      <c r="AP2" s="68"/>
+      <c r="AQ2" s="68"/>
+      <c r="AR2" s="68"/>
+      <c r="AS2" s="68"/>
+      <c r="AT2" s="68"/>
+      <c r="AU2" s="68"/>
+      <c r="AV2" s="68"/>
+      <c r="AW2" s="68"/>
+      <c r="AX2" s="68"/>
+      <c r="AY2" s="68"/>
+      <c r="AZ2" s="68"/>
+      <c r="BA2" s="68"/>
+      <c r="BB2" s="68"/>
+      <c r="BC2" s="68"/>
+      <c r="BD2" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="BE2" s="57"/>
-      <c r="BF2" s="57"/>
-      <c r="BG2" s="57"/>
-      <c r="BH2" s="57"/>
-      <c r="BI2" s="57"/>
-      <c r="BJ2" s="57"/>
-      <c r="BK2" s="57"/>
-      <c r="BL2" s="57"/>
-      <c r="BM2" s="57"/>
-      <c r="BN2" s="57"/>
-      <c r="BO2" s="57"/>
-      <c r="BP2" s="57"/>
-      <c r="BQ2" s="57"/>
-      <c r="BR2" s="57"/>
-      <c r="BS2" s="57"/>
-      <c r="BT2" s="57" t="s">
+      <c r="BE2" s="68"/>
+      <c r="BF2" s="68"/>
+      <c r="BG2" s="68"/>
+      <c r="BH2" s="68"/>
+      <c r="BI2" s="68"/>
+      <c r="BJ2" s="68"/>
+      <c r="BK2" s="68"/>
+      <c r="BL2" s="68"/>
+      <c r="BM2" s="68"/>
+      <c r="BN2" s="68"/>
+      <c r="BO2" s="68"/>
+      <c r="BP2" s="68"/>
+      <c r="BQ2" s="68"/>
+      <c r="BR2" s="68"/>
+      <c r="BS2" s="68"/>
+      <c r="BT2" s="68" t="s">
         <v>77</v>
       </c>
-      <c r="BU2" s="57"/>
-      <c r="BV2" s="57"/>
-      <c r="BW2" s="57"/>
-      <c r="BX2" s="57"/>
-      <c r="BY2" s="57"/>
-      <c r="BZ2" s="57"/>
-      <c r="CA2" s="57"/>
-      <c r="CB2" s="57"/>
-      <c r="CC2" s="57"/>
-      <c r="CD2" s="57"/>
-      <c r="CE2" s="57"/>
-      <c r="CF2" s="57"/>
-      <c r="CG2" s="57"/>
-      <c r="CH2" s="57"/>
-      <c r="CI2" s="57"/>
+      <c r="BU2" s="68"/>
+      <c r="BV2" s="68"/>
+      <c r="BW2" s="68"/>
+      <c r="BX2" s="68"/>
+      <c r="BY2" s="68"/>
+      <c r="BZ2" s="68"/>
+      <c r="CA2" s="68"/>
+      <c r="CB2" s="68"/>
+      <c r="CC2" s="68"/>
+      <c r="CD2" s="68"/>
+      <c r="CE2" s="68"/>
+      <c r="CF2" s="68"/>
+      <c r="CG2" s="68"/>
+      <c r="CH2" s="68"/>
+      <c r="CI2" s="68"/>
       <c r="CJ2" s="50"/>
     </row>
     <row r="3" spans="1:105" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F3" s="55"/>
       <c r="G3" s="18"/>
-      <c r="H3" s="58" t="s">
+      <c r="H3" s="69" t="s">
         <v>78</v>
       </c>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="61" t="s">
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="M3" s="62"/>
-      <c r="N3" s="62"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="64" t="s">
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="72" t="s">
         <v>80</v>
       </c>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
+      <c r="Q3" s="72"/>
+      <c r="R3" s="72"/>
       <c r="S3" s="19"/>
-      <c r="T3" s="65" t="s">
+      <c r="T3" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="U3" s="66"/>
-      <c r="V3" s="66"/>
-      <c r="W3" s="67"/>
-      <c r="X3" s="68" t="s">
+      <c r="U3" s="64"/>
+      <c r="V3" s="64"/>
+      <c r="W3" s="73"/>
+      <c r="X3" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="Y3" s="69"/>
-      <c r="Z3" s="69"/>
-      <c r="AA3" s="70"/>
-      <c r="AB3" s="76" t="s">
+      <c r="Y3" s="75"/>
+      <c r="Z3" s="75"/>
+      <c r="AA3" s="76"/>
+      <c r="AB3" s="79" t="s">
         <v>79</v>
       </c>
-      <c r="AC3" s="80"/>
-      <c r="AD3" s="80"/>
-      <c r="AE3" s="74"/>
-      <c r="AF3" s="81" t="s">
+      <c r="AC3" s="83"/>
+      <c r="AD3" s="83"/>
+      <c r="AE3" s="77"/>
+      <c r="AF3" s="84" t="s">
         <v>80</v>
       </c>
-      <c r="AG3" s="82"/>
-      <c r="AH3" s="82"/>
-      <c r="AI3" s="83"/>
-      <c r="AJ3" s="84" t="s">
+      <c r="AG3" s="85"/>
+      <c r="AH3" s="85"/>
+      <c r="AI3" s="86"/>
+      <c r="AJ3" s="87" t="s">
         <v>81</v>
       </c>
-      <c r="AK3" s="85"/>
-      <c r="AL3" s="85"/>
-      <c r="AM3" s="85"/>
-      <c r="AN3" s="86" t="s">
+      <c r="AK3" s="88"/>
+      <c r="AL3" s="88"/>
+      <c r="AM3" s="88"/>
+      <c r="AN3" s="89" t="s">
         <v>78</v>
       </c>
-      <c r="AO3" s="87"/>
-      <c r="AP3" s="87"/>
-      <c r="AQ3" s="88"/>
-      <c r="AR3" s="61" t="s">
+      <c r="AO3" s="66"/>
+      <c r="AP3" s="66"/>
+      <c r="AQ3" s="67"/>
+      <c r="AR3" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="AS3" s="62"/>
-      <c r="AT3" s="62"/>
-      <c r="AU3" s="63"/>
-      <c r="AV3" s="71" t="s">
+      <c r="AS3" s="58"/>
+      <c r="AT3" s="58"/>
+      <c r="AU3" s="59"/>
+      <c r="AV3" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="AW3" s="72"/>
-      <c r="AX3" s="72"/>
-      <c r="AY3" s="73"/>
-      <c r="AZ3" s="65" t="s">
+      <c r="AW3" s="61"/>
+      <c r="AX3" s="61"/>
+      <c r="AY3" s="62"/>
+      <c r="AZ3" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="BA3" s="66"/>
-      <c r="BB3" s="66"/>
-      <c r="BC3" s="66"/>
-      <c r="BD3" s="87" t="s">
+      <c r="BA3" s="64"/>
+      <c r="BB3" s="64"/>
+      <c r="BC3" s="64"/>
+      <c r="BD3" s="66" t="s">
         <v>78</v>
       </c>
-      <c r="BE3" s="87"/>
-      <c r="BF3" s="87"/>
-      <c r="BG3" s="88"/>
-      <c r="BH3" s="61" t="s">
+      <c r="BE3" s="66"/>
+      <c r="BF3" s="66"/>
+      <c r="BG3" s="67"/>
+      <c r="BH3" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="BI3" s="62"/>
-      <c r="BJ3" s="62"/>
-      <c r="BK3" s="63"/>
-      <c r="BL3" s="71" t="s">
+      <c r="BI3" s="58"/>
+      <c r="BJ3" s="58"/>
+      <c r="BK3" s="59"/>
+      <c r="BL3" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="BM3" s="72"/>
-      <c r="BN3" s="72"/>
-      <c r="BO3" s="73"/>
-      <c r="BP3" s="65" t="s">
+      <c r="BM3" s="61"/>
+      <c r="BN3" s="61"/>
+      <c r="BO3" s="62"/>
+      <c r="BP3" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="BQ3" s="66"/>
-      <c r="BR3" s="66"/>
-      <c r="BS3" s="66"/>
-      <c r="BT3" s="87" t="s">
+      <c r="BQ3" s="64"/>
+      <c r="BR3" s="64"/>
+      <c r="BS3" s="64"/>
+      <c r="BT3" s="66" t="s">
         <v>78</v>
       </c>
-      <c r="BU3" s="87"/>
-      <c r="BV3" s="87"/>
-      <c r="BW3" s="88"/>
-      <c r="BX3" s="61" t="s">
+      <c r="BU3" s="66"/>
+      <c r="BV3" s="66"/>
+      <c r="BW3" s="67"/>
+      <c r="BX3" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="BY3" s="62"/>
-      <c r="BZ3" s="62"/>
-      <c r="CA3" s="63"/>
-      <c r="CB3" s="71" t="s">
+      <c r="BY3" s="58"/>
+      <c r="BZ3" s="58"/>
+      <c r="CA3" s="59"/>
+      <c r="CB3" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="CC3" s="72"/>
-      <c r="CD3" s="72"/>
-      <c r="CE3" s="73"/>
-      <c r="CF3" s="65" t="s">
+      <c r="CC3" s="61"/>
+      <c r="CD3" s="61"/>
+      <c r="CE3" s="62"/>
+      <c r="CF3" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="CG3" s="66"/>
-      <c r="CH3" s="66"/>
-      <c r="CI3" s="89"/>
+      <c r="CG3" s="64"/>
+      <c r="CH3" s="64"/>
+      <c r="CI3" s="65"/>
       <c r="CJ3" s="16"/>
     </row>
     <row r="4" spans="1:105" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -9719,7 +9731,7 @@
         <v>524</v>
       </c>
       <c r="G16" s="34">
-        <v>1979</v>
+        <v>1752</v>
       </c>
       <c r="H16" s="35">
         <v>2489</v>
@@ -9819,67 +9831,67 @@
       </c>
       <c r="AN16" s="31">
         <f>(X16*100)/G16</f>
-        <v>23.900960080848915</v>
+        <v>26.99771689497717</v>
       </c>
       <c r="AO16" s="38">
         <f>(Y16*100)/G16</f>
-        <v>12.531581606872157</v>
+        <v>14.155251141552512</v>
       </c>
       <c r="AP16" s="31">
         <f>(Z16*100)/G16</f>
-        <v>8.5901970692268819</v>
+        <v>9.7031963470319642</v>
       </c>
       <c r="AQ16" s="37">
         <f>(AA16*100)/G16</f>
-        <v>6.872157655381506</v>
+        <v>7.762557077625571</v>
       </c>
       <c r="AR16" s="38">
         <f>(AB16*100)/G16</f>
-        <v>35.573521980798382</v>
+        <v>40.182648401826484</v>
       </c>
       <c r="AS16" s="38">
         <f>(AC16*100)/G16</f>
-        <v>18.393127842344619</v>
+        <v>20.776255707762559</v>
       </c>
       <c r="AT16" s="31">
         <f>(AD16*100)/G16</f>
-        <v>12.379989893885801</v>
+        <v>13.984018264840183</v>
       </c>
       <c r="AU16" s="37">
         <f>(AE16*100)/G16</f>
-        <v>10.207175341081355</v>
+        <v>11.529680365296803</v>
       </c>
       <c r="AV16" s="38">
         <f>(AF16*100)/G16</f>
-        <v>44.770085901970695</v>
+        <v>50.570776255707763</v>
       </c>
       <c r="AW16" s="38">
         <f>(AG16*100)/G16</f>
-        <v>23.547246083880747</v>
+        <v>26.598173515981735</v>
       </c>
       <c r="AX16" s="31">
         <f>(AH16*100)/G16</f>
-        <v>14.906518443658413</v>
+        <v>16.837899543378995</v>
       </c>
       <c r="AY16" s="37">
         <f>(AI16*100)/G16</f>
-        <v>12.127337038908539</v>
+        <v>13.698630136986301</v>
       </c>
       <c r="AZ16" s="38">
         <f>(AJ16*100)/G16</f>
-        <v>90.146538655886815</v>
+        <v>101.82648401826484</v>
       </c>
       <c r="BA16" s="38">
         <f>(AK16*100)/G16</f>
-        <v>68.923698837796863</v>
+        <v>77.853881278538807</v>
       </c>
       <c r="BB16" s="31">
         <f>(AL16*100)/G16</f>
-        <v>51.035876705406771</v>
+        <v>57.648401826484019</v>
       </c>
       <c r="BC16" s="37">
         <f>(AM16*100)/G16</f>
-        <v>36.331480545730166</v>
+        <v>41.038812785388124</v>
       </c>
       <c r="BD16" s="31">
         <f t="shared" ref="BD16:BD17" si="33">(X16*100)/H16</f>
@@ -9947,67 +9959,67 @@
       </c>
       <c r="BT16" s="31">
         <f>H16/G16</f>
-        <v>1.2577059120768064</v>
+        <v>1.4206621004566211</v>
       </c>
       <c r="BU16" s="31">
         <f>I16/G16</f>
-        <v>0.45831227892875187</v>
+        <v>0.51769406392694062</v>
       </c>
       <c r="BV16" s="31">
         <f>J16/G16</f>
-        <v>0.25669530065689744</v>
+        <v>0.28995433789954339</v>
       </c>
       <c r="BW16" s="37">
         <f>K16/G16</f>
-        <v>0.19454269833249116</v>
+        <v>0.21974885844748859</v>
       </c>
       <c r="BX16" s="31">
         <f>L16/G16</f>
-        <v>2.8231430015159171</v>
+        <v>3.1889269406392695</v>
       </c>
       <c r="BY16" s="31">
         <f>M16/G16</f>
-        <v>0.91763516927741284</v>
+        <v>1.0365296803652968</v>
       </c>
       <c r="BZ16" s="31">
         <f>N16/G16</f>
-        <v>0.43658413340070745</v>
+        <v>0.49315068493150682</v>
       </c>
       <c r="CA16" s="37">
         <f>O16/G16</f>
-        <v>0.30722587165234966</v>
+        <v>0.34703196347031962</v>
       </c>
       <c r="CB16" s="31">
         <f>P16/G16</f>
-        <v>4.8842849924204144</v>
+        <v>5.5171232876712333</v>
       </c>
       <c r="CC16" s="31">
         <f>Q16/G16</f>
-        <v>1.5224861040929762</v>
+        <v>1.7197488584474885</v>
       </c>
       <c r="CD16" s="31">
         <f>R16/G16</f>
-        <v>0.6760990399191511</v>
+        <v>0.76369863013698636</v>
       </c>
       <c r="CE16" s="37">
         <f>S16/G16</f>
-        <v>0.39717028802425469</v>
+        <v>0.44863013698630139</v>
       </c>
       <c r="CF16" s="31">
         <f>T16/G16</f>
-        <v>47.811015664477011</v>
+        <v>54.00570776255708</v>
       </c>
       <c r="CG16" s="31">
         <f>U16/G16</f>
-        <v>25.119757453259222</v>
+        <v>28.374429223744293</v>
       </c>
       <c r="CH16" s="31">
         <f>V16/G16</f>
-        <v>12.879231935320869</v>
+        <v>14.547945205479452</v>
       </c>
       <c r="CI16" s="37">
         <f>W16/G16</f>
-        <v>7.4643759474482065</v>
+        <v>8.4315068493150687</v>
       </c>
       <c r="CJ16" s="39" t="s">
         <v>93</v>
@@ -11175,7 +11187,7 @@
         <v>685</v>
       </c>
       <c r="G21" s="43">
-        <v>1940</v>
+        <v>2571</v>
       </c>
       <c r="H21" s="31">
         <v>4117</v>
@@ -11275,67 +11287,67 @@
       </c>
       <c r="AN21" s="31">
         <f t="shared" ref="AN21" si="97">(X21*100)/G21</f>
-        <v>31.030927835051546</v>
+        <v>23.415013613380008</v>
       </c>
       <c r="AO21" s="38">
         <f t="shared" ref="AO21" si="98">(Y21*100)/G21</f>
-        <v>18.865979381443299</v>
+        <v>14.235705950991832</v>
       </c>
       <c r="AP21" s="31">
         <f t="shared" ref="AP21" si="99">(Z21*100)/G21</f>
-        <v>15.103092783505154</v>
+        <v>11.396343835083625</v>
       </c>
       <c r="AQ21" s="37">
         <f t="shared" ref="AQ21" si="100">(AA21*100)/G21</f>
-        <v>10.618556701030927</v>
+        <v>8.0124465188642553</v>
       </c>
       <c r="AR21" s="38">
         <f t="shared" ref="AR21" si="101">(AB21*100)/G21</f>
-        <v>43.865979381443296</v>
+        <v>33.099961104628548</v>
       </c>
       <c r="AS21" s="38">
         <f t="shared" ref="AS21" si="102">(AC21*100)/G21</f>
-        <v>27.835051546391753</v>
+        <v>21.003500583430572</v>
       </c>
       <c r="AT21" s="31">
         <f t="shared" ref="AT21" si="103">(AD21*100)/G21</f>
-        <v>20.979381443298969</v>
+        <v>15.830416180474524</v>
       </c>
       <c r="AU21" s="37">
         <f t="shared" ref="AU21" si="104">(AE21*100)/G21</f>
-        <v>13.969072164948454</v>
+        <v>10.540645663166083</v>
       </c>
       <c r="AV21" s="38">
         <f t="shared" ref="AV21" si="105">(AF21*100)/G21</f>
-        <v>52.010309278350519</v>
+        <v>39.245429793854534</v>
       </c>
       <c r="AW21" s="38">
         <f t="shared" ref="AW21" si="106">(AG21*100)/G21</f>
-        <v>35</v>
+        <v>26.409957215091403</v>
       </c>
       <c r="AX21" s="31">
         <f t="shared" ref="AX21" si="107">(AH21*100)/G21</f>
-        <v>26.855670103092784</v>
+        <v>20.264488525865421</v>
       </c>
       <c r="AY21" s="37">
         <f t="shared" ref="AY21" si="108">(AI21*100)/G21</f>
-        <v>19.020618556701031</v>
+        <v>14.352392065344224</v>
       </c>
       <c r="AZ21" s="38">
         <f t="shared" ref="AZ21" si="109">(AJ21*100)/G21</f>
-        <v>75.30927835051547</v>
+        <v>56.826137689614939</v>
       </c>
       <c r="BA21" s="38">
         <f t="shared" ref="BA21" si="110">(AK21*100)/G21</f>
-        <v>53.092783505154642</v>
+        <v>40.062232594321273</v>
       </c>
       <c r="BB21" s="31">
         <f t="shared" ref="BB21" si="111">(AL21*100)/G21</f>
-        <v>40.567010309278352</v>
+        <v>30.610657331777517</v>
       </c>
       <c r="BC21" s="37">
         <f t="shared" ref="BC21" si="112">(AM21*100)/G21</f>
-        <v>30.206185567010309</v>
+        <v>22.792687670167251</v>
       </c>
       <c r="BD21" s="31">
         <f t="shared" ref="BD21" si="113">(X21*100)/H21</f>
@@ -11403,83 +11415,252 @@
       </c>
       <c r="BT21" s="31">
         <f t="shared" ref="BT21" si="129">H21/G21</f>
-        <v>2.1221649484536083</v>
+        <v>1.6013224426293271</v>
       </c>
       <c r="BU21" s="31">
         <f t="shared" ref="BU21" si="130">I21/G21</f>
-        <v>0.90463917525773196</v>
+        <v>0.68261376896149362</v>
       </c>
       <c r="BV21" s="31">
         <f t="shared" ref="BV21" si="131">J21/G21</f>
-        <v>0.71597938144329898</v>
+        <v>0.54025670945157522</v>
       </c>
       <c r="BW21" s="37">
         <f t="shared" ref="BW21" si="132">K21/G21</f>
-        <v>0.3804123711340206</v>
+        <v>0.28704784130688449</v>
       </c>
       <c r="BX21" s="31">
         <f t="shared" ref="BX21" si="133">L21/G21</f>
-        <v>3.6381443298969072</v>
+        <v>2.7452353169972774</v>
       </c>
       <c r="BY21" s="31">
         <f t="shared" ref="BY21" si="134">M21/G21</f>
-        <v>1.5984536082474228</v>
+        <v>1.2061454686892259</v>
       </c>
       <c r="BZ21" s="31">
         <f t="shared" ref="BZ21" si="135">N21/G21</f>
-        <v>1.0768041237113402</v>
+        <v>0.81252430960715671</v>
       </c>
       <c r="CA21" s="37">
         <f t="shared" ref="CA21" si="136">O21/G21</f>
-        <v>0.59072164948453609</v>
+        <v>0.44574095682613768</v>
       </c>
       <c r="CB21" s="31">
         <f t="shared" ref="CB21" si="137">P21/G21</f>
-        <v>6.0226804123711339</v>
+        <v>4.544535200311163</v>
       </c>
       <c r="CC21" s="31">
         <f t="shared" ref="CC21" si="138">Q21/G21</f>
-        <v>2.6572164948453607</v>
+        <v>2.0050563982886036</v>
       </c>
       <c r="CD21" s="31">
         <f t="shared" ref="CD21" si="139">R21/G21</f>
-        <v>1.6154639175257732</v>
+        <v>1.2189809412679891</v>
       </c>
       <c r="CE21" s="37">
         <f t="shared" ref="CE21" si="140">S21/G21</f>
-        <v>0.92628865979381447</v>
+        <v>0.69894982497082847</v>
       </c>
       <c r="CF21" s="31">
         <f t="shared" ref="CF21" si="141">T21/G21</f>
-        <v>30.537628865979382</v>
+        <v>23.042784908595877</v>
       </c>
       <c r="CG21" s="31">
         <f t="shared" ref="CG21" si="142">U21/G21</f>
-        <v>14.485567010309278</v>
+        <v>10.930377285103074</v>
       </c>
       <c r="CH21" s="31">
         <f t="shared" ref="CH21" si="143">V21/G21</f>
-        <v>7.2051546391752579</v>
+        <v>5.4367950213924541</v>
       </c>
       <c r="CI21" s="37">
         <f t="shared" ref="CI21" si="144">W21/G21</f>
-        <v>3.8226804123711342</v>
+        <v>2.884480746791132</v>
       </c>
       <c r="CJ21" s="44" t="s">
         <v>93</v>
       </c>
     </row>
+    <row r="24" spans="1:105" x14ac:dyDescent="0.25">
+      <c r="A24" s="20"/>
+      <c r="B24" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="G24" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>1993</v>
+      </c>
+      <c r="I24" s="20" t="s">
+        <v>1994</v>
+      </c>
+      <c r="J24" s="22" t="s">
+        <v>1995</v>
+      </c>
+      <c r="K24" s="20" t="s">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:105" x14ac:dyDescent="0.25">
+      <c r="A25" s="30">
+        <v>1</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="32">
+        <v>1314</v>
+      </c>
+      <c r="D25" s="32">
+        <v>4601</v>
+      </c>
+      <c r="E25" s="33">
+        <v>504</v>
+      </c>
+      <c r="F25" s="33">
+        <v>524</v>
+      </c>
+      <c r="G25" s="34">
+        <v>1757</v>
+      </c>
+      <c r="H25" s="35">
+        <v>37688</v>
+      </c>
+      <c r="I25" s="32">
+        <v>21627</v>
+      </c>
+    </row>
+    <row r="26" spans="1:105" x14ac:dyDescent="0.25">
+      <c r="A26" s="30">
+        <v>2</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="32">
+        <v>10051</v>
+      </c>
+      <c r="D26" s="32">
+        <v>5255</v>
+      </c>
+      <c r="E26" s="33">
+        <v>3671</v>
+      </c>
+      <c r="F26" s="33">
+        <v>4477</v>
+      </c>
+      <c r="G26" s="34">
+        <v>20846</v>
+      </c>
+      <c r="H26" s="35">
+        <v>3288</v>
+      </c>
+      <c r="I26" s="32">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="27" spans="1:105" x14ac:dyDescent="0.25">
+      <c r="A27" s="30">
+        <v>3</v>
+      </c>
+      <c r="B27" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="38">
+        <v>1362</v>
+      </c>
+      <c r="D27" s="38">
+        <v>1630</v>
+      </c>
+      <c r="E27" s="42">
+        <v>256</v>
+      </c>
+      <c r="F27" s="42">
+        <v>280</v>
+      </c>
+      <c r="G27" s="43">
+        <v>978</v>
+      </c>
+      <c r="H27" s="31">
+        <v>463</v>
+      </c>
+      <c r="I27" s="38">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:105" x14ac:dyDescent="0.25">
+      <c r="A28" s="30">
+        <v>4</v>
+      </c>
+      <c r="B28" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="31">
+        <v>564</v>
+      </c>
+      <c r="D28" s="31">
+        <v>2189</v>
+      </c>
+      <c r="E28" s="42">
+        <v>243</v>
+      </c>
+      <c r="F28" s="42">
+        <v>336</v>
+      </c>
+      <c r="G28" s="43">
+        <v>1035</v>
+      </c>
+      <c r="H28" s="31">
+        <v>377</v>
+      </c>
+      <c r="I28" s="31">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="29" spans="1:105" x14ac:dyDescent="0.25">
+      <c r="A29" s="30">
+        <v>5</v>
+      </c>
+      <c r="B29" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" s="31">
+        <v>3018</v>
+      </c>
+      <c r="D29" s="31">
+        <v>14931</v>
+      </c>
+      <c r="E29" s="42">
+        <v>576</v>
+      </c>
+      <c r="F29" s="42">
+        <v>685</v>
+      </c>
+      <c r="G29" s="43">
+        <v>2571</v>
+      </c>
+      <c r="H29" s="31">
+        <v>11676</v>
+      </c>
+      <c r="I29" s="31">
+        <v>5121</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="BX3:CA3"/>
-    <mergeCell ref="CB3:CE3"/>
-    <mergeCell ref="CF3:CI3"/>
-    <mergeCell ref="AZ3:BC3"/>
-    <mergeCell ref="BD3:BG3"/>
-    <mergeCell ref="BH3:BK3"/>
-    <mergeCell ref="BL3:BO3"/>
-    <mergeCell ref="BP3:BS3"/>
-    <mergeCell ref="BT3:BW3"/>
     <mergeCell ref="BT2:CI2"/>
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="L3:O3"/>
@@ -11496,6 +11677,15 @@
     <mergeCell ref="AJ3:AM3"/>
     <mergeCell ref="AN3:AQ3"/>
     <mergeCell ref="AR3:AU3"/>
+    <mergeCell ref="BX3:CA3"/>
+    <mergeCell ref="CB3:CE3"/>
+    <mergeCell ref="CF3:CI3"/>
+    <mergeCell ref="AZ3:BC3"/>
+    <mergeCell ref="BD3:BG3"/>
+    <mergeCell ref="BH3:BK3"/>
+    <mergeCell ref="BL3:BO3"/>
+    <mergeCell ref="BP3:BS3"/>
+    <mergeCell ref="BT3:BW3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
refactor count occurences number
</commit_message>
<xml_diff>
--- a/results/keyclasses_results.xlsx
+++ b/results/keyclasses_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="overview" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1995" uniqueCount="1977">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2011" uniqueCount="1993">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -5952,6 +5952,54 @@
   </si>
   <si>
     <t>4 occ</t>
+  </si>
+  <si>
+    <t>5 occ</t>
+  </si>
+  <si>
+    <t>6 occ</t>
+  </si>
+  <si>
+    <t>7 occ</t>
+  </si>
+  <si>
+    <t>8 occ</t>
+  </si>
+  <si>
+    <t>9 occ</t>
+  </si>
+  <si>
+    <t>10 occ</t>
+  </si>
+  <si>
+    <t>11 occ</t>
+  </si>
+  <si>
+    <t>12 occ</t>
+  </si>
+  <si>
+    <t>13 occ</t>
+  </si>
+  <si>
+    <t>14 occ</t>
+  </si>
+  <si>
+    <t>15 occ</t>
+  </si>
+  <si>
+    <t>16 occ</t>
+  </si>
+  <si>
+    <t>17 occ</t>
+  </si>
+  <si>
+    <t>18 occ</t>
+  </si>
+  <si>
+    <t>19 occ</t>
+  </si>
+  <si>
+    <t>20 occ</t>
   </si>
 </sst>
 </file>
@@ -6497,7 +6545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -7100,10 +7148,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K7"/>
+  <dimension ref="A2:AA7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7113,7 +7161,7 @@
     <col min="7" max="7" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
       <c r="B2" s="14" t="s">
         <v>71</v>
@@ -7145,8 +7193,56 @@
       <c r="K2" s="14" t="s">
         <v>1976</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="16" t="s">
+        <v>1977</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>1978</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>1979</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>1980</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>1981</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>1982</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>1983</v>
+      </c>
+      <c r="S2" s="14" t="s">
+        <v>1984</v>
+      </c>
+      <c r="T2" s="16" t="s">
+        <v>1985</v>
+      </c>
+      <c r="U2" s="14" t="s">
+        <v>1986</v>
+      </c>
+      <c r="V2" s="16" t="s">
+        <v>1987</v>
+      </c>
+      <c r="W2" s="14" t="s">
+        <v>1988</v>
+      </c>
+      <c r="X2" s="16" t="s">
+        <v>1989</v>
+      </c>
+      <c r="Y2" s="14" t="s">
+        <v>1990</v>
+      </c>
+      <c r="Z2" s="16" t="s">
+        <v>1991</v>
+      </c>
+      <c r="AA2" s="14" t="s">
+        <v>1992</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="18">
         <v>1</v>
       </c>
@@ -7180,8 +7276,56 @@
       <c r="K3" s="19">
         <v>10315</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>8378</v>
+      </c>
+      <c r="M3">
+        <v>6545</v>
+      </c>
+      <c r="N3">
+        <v>5387</v>
+      </c>
+      <c r="O3">
+        <v>4606</v>
+      </c>
+      <c r="P3">
+        <v>4079</v>
+      </c>
+      <c r="Q3">
+        <v>3827</v>
+      </c>
+      <c r="R3">
+        <v>3674</v>
+      </c>
+      <c r="S3">
+        <v>3575</v>
+      </c>
+      <c r="T3">
+        <v>3515</v>
+      </c>
+      <c r="U3">
+        <v>3490</v>
+      </c>
+      <c r="V3">
+        <v>3465</v>
+      </c>
+      <c r="W3">
+        <v>3414</v>
+      </c>
+      <c r="X3">
+        <v>3405</v>
+      </c>
+      <c r="Y3">
+        <v>3389</v>
+      </c>
+      <c r="Z3">
+        <v>3380</v>
+      </c>
+      <c r="AA3">
+        <v>3376</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="18">
         <v>2</v>
       </c>
@@ -7215,8 +7359,56 @@
       <c r="K4" s="19">
         <v>51837</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>29211</v>
+      </c>
+      <c r="M4">
+        <v>22678</v>
+      </c>
+      <c r="N4">
+        <v>10607</v>
+      </c>
+      <c r="O4">
+        <v>8504</v>
+      </c>
+      <c r="P4">
+        <v>3611</v>
+      </c>
+      <c r="Q4">
+        <v>2909</v>
+      </c>
+      <c r="R4">
+        <v>778</v>
+      </c>
+      <c r="S4">
+        <v>362</v>
+      </c>
+      <c r="T4">
+        <v>245</v>
+      </c>
+      <c r="U4">
+        <v>239</v>
+      </c>
+      <c r="V4">
+        <v>239</v>
+      </c>
+      <c r="W4">
+        <v>217</v>
+      </c>
+      <c r="X4">
+        <v>210</v>
+      </c>
+      <c r="Y4">
+        <v>208</v>
+      </c>
+      <c r="Z4">
+        <v>208</v>
+      </c>
+      <c r="AA4">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
         <v>3</v>
       </c>
@@ -7251,7 +7443,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="18">
         <v>4</v>
       </c>
@@ -7286,7 +7478,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="18">
         <v>5</v>
       </c>
@@ -7302,23 +7494,71 @@
       <c r="E7" s="24">
         <v>685</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7">
         <v>576</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7">
         <v>1617</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7">
         <v>11684</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7">
         <v>5155</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7">
         <v>3134</v>
       </c>
-      <c r="K7" s="19">
+      <c r="K7">
         <v>1797</v>
+      </c>
+      <c r="L7">
+        <v>1305</v>
+      </c>
+      <c r="M7">
+        <v>999</v>
+      </c>
+      <c r="N7">
+        <v>892</v>
+      </c>
+      <c r="O7">
+        <v>775</v>
+      </c>
+      <c r="P7">
+        <v>673</v>
+      </c>
+      <c r="Q7">
+        <v>586</v>
+      </c>
+      <c r="R7">
+        <v>553</v>
+      </c>
+      <c r="S7">
+        <v>476</v>
+      </c>
+      <c r="T7">
+        <v>409</v>
+      </c>
+      <c r="U7">
+        <v>382</v>
+      </c>
+      <c r="V7">
+        <v>376</v>
+      </c>
+      <c r="W7">
+        <v>282</v>
+      </c>
+      <c r="X7">
+        <v>281</v>
+      </c>
+      <c r="Y7">
+        <v>259</v>
+      </c>
+      <c r="Z7">
+        <v>149</v>
+      </c>
+      <c r="AA7">
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>